<commit_message>
Changed colouring on graph and updated files
</commit_message>
<xml_diff>
--- a/1-Foundations-Data-Data-Everywhere/Exercises/1-analysis-monthly-sales.xlsx
+++ b/1-Foundations-Data-Data-Everywhere/Exercises/1-analysis-monthly-sales.xlsx
@@ -173,9 +173,7 @@
           <c:spPr>
             <a:ln cmpd="sng" w="38100">
               <a:solidFill>
-                <a:srgbClr val="0000FF">
-                  <a:alpha val="100000"/>
-                </a:srgbClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -195,8 +193,8 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1084648582"/>
-        <c:axId val="1693348049"/>
+        <c:axId val="1736543362"/>
+        <c:axId val="282870887"/>
       </c:lineChart>
       <c:areaChart>
         <c:ser>
@@ -209,13 +207,13 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FF0000">
+              <a:srgbClr val="6AA84F">
                 <a:alpha val="30000"/>
               </a:srgbClr>
             </a:solidFill>
             <a:ln cmpd="sng" w="9525">
               <a:solidFill>
-                <a:srgbClr val="FF0000">
+                <a:srgbClr val="6AA84F">
                   <a:alpha val="0"/>
                 </a:srgbClr>
               </a:solidFill>
@@ -233,11 +231,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1084648582"/>
-        <c:axId val="1693348049"/>
+        <c:axId val="1736543362"/>
+        <c:axId val="282870887"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1084648582"/>
+        <c:axId val="1736543362"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -289,10 +287,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1693348049"/>
+        <c:crossAx val="282870887"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1693348049"/>
+        <c:axId val="282870887"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -367,7 +365,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1084648582"/>
+        <c:crossAx val="1736543362"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>

</xml_diff>